<commit_message>
added in the custom cheatsheet for cheatsheet page.
</commit_message>
<xml_diff>
--- a/RB.xlsx
+++ b/RB.xlsx
@@ -891,7 +891,7 @@
   <dimension ref="A1:B177"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,12 +919,12 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>